<commit_message>
refactor: filled user stories/backlog skeletons
</commit_message>
<xml_diff>
--- a/Product Backlog-1.xlsx
+++ b/Product Backlog-1.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamal\Desktop\Schoolwork\Summer 2025\ITSC 3155 (Software Engineering)\Group Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE2CE0-DB5C-4E4B-BF4B-526C6C13CA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="14424" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -37,49 +46,87 @@
     <t>SPRINT #</t>
   </si>
   <si>
-    <t>Feature 1</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Online Ordering Interface</t>
+  </si>
+  <si>
+    <t>Develop customer-facing web/API platform</t>
+  </si>
+  <si>
+    <t>Enable guest checkout for new users</t>
+  </si>
+  <si>
+    <t>Design menu display with dish metadata</t>
+  </si>
+  <si>
+    <t>Provide takeout and delivery selection options</t>
+  </si>
+  <si>
+    <t>Integrate real-time order tracking system</t>
+  </si>
+  <si>
+    <t>Setup multi-method payment processing</t>
+  </si>
+  <si>
+    <t>Create role-based dashboards (staff/chef/admin)</t>
+  </si>
+  <si>
+    <t>Build real-time kitchen order display system</t>
+  </si>
+  <si>
+    <t>Develop admin analytics dashboard</t>
+  </si>
+  <si>
+    <t>Add customer review/rating module</t>
+  </si>
+  <si>
+    <t>Implement feedback reporting and analysis tools</t>
+  </si>
+  <si>
+    <t>Enable coupon and promo code engine</t>
+  </si>
+  <si>
+    <t>Build promotion management dashboard</t>
+  </si>
+  <si>
+    <t>Setup data analytics and sales reporting tools</t>
+  </si>
+  <si>
+    <t>Create integrated training resources for staff</t>
+  </si>
+  <si>
+    <t>Provide comprehensive system documentation repo</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
@@ -283,61 +330,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,27 +372,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fffff2cc"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffcfe2f3"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffbfbfbf"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFCFE2F3"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFBFBFBF"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -569,7 +652,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -587,7 +670,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -616,7 +699,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -641,7 +724,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -666,7 +749,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -691,7 +774,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -716,7 +799,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -741,7 +824,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -766,7 +849,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -791,7 +874,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -816,7 +899,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -829,9 +912,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -848,7 +937,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -866,7 +955,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -891,7 +980,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -916,7 +1005,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +1030,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -966,7 +1055,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -991,7 +1080,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1016,7 +1105,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1041,7 +1130,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1066,7 +1155,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1091,7 +1180,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1104,9 +1193,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1120,7 +1215,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1138,7 +1233,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1167,7 +1262,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +1287,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1217,7 +1312,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1337,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1267,7 +1362,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1292,7 +1387,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1412,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1342,7 +1437,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1367,7 +1462,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1380,180 +1475,421 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="42.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.44140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="s" s="5">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="9">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="10">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s" s="10">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="11">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="C4" s="6">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="12">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="12">
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="13">
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="15"/>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="15"/>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="8">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="15"/>
+    <row r="8" spans="1:6" ht="15" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15"/>
+    <row r="9" spans="1:6" ht="15" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
+    <row r="10" spans="1:6" ht="15" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="15"/>
+    <row r="11" spans="1:6" ht="15" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="8">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="15"/>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="15"/>
+    <row r="13" spans="1:6" ht="15" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="15"/>
+    <row r="14" spans="1:6" ht="15" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="15"/>
+    <row r="15" spans="1:6" ht="15" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15"/>
+    <row r="16" spans="1:6" ht="15" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="8">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1">
+      <c r="A18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1561,15 +1897,15 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B7:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E4 D7:E15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E20" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>